<commit_message>
some updates in final project
</commit_message>
<xml_diff>
--- a/final_project/BB_Traj_V2/BB_Traj_V2/DataBase/PRODAS-MODIFICADO.xlsx
+++ b/final_project/BB_Traj_V2/BB_Traj_V2/DataBase/PRODAS-MODIFICADO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99f6e88dae47a7e2/Área de Trabalho/Nova pasta/tcc/TCC/PYTHON/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99f6e88dae47a7e2/Área de Trabalho/mestrado_ime/scientf-comp-mecheng-ime/final_project/BB_Traj_V2/BB_Traj_V2/DataBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_7A41F6A1736A9189BE186DD895B26B001FF3C504" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E3D8814-C04A-49DA-82FE-F27352CCFA47}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_7A41F6A1736A9189BE186DD895B26B001FF3C504" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF27DA09-2CF7-4AE3-94F8-301562CAD170}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,31 +172,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="prodas" displayName="prodas" ref="A1:P31" totalsRowShown="0">
-  <autoFilter ref="A1:P31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Mach"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Cx0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cx2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cd2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Cx4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cla"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CNa"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="CNa3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cmag_f"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cma"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Cma3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Cma5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cmq"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Cmq2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cspin"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Cld"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,7 +474,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,8 +2417,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>